<commit_message>
Frontend update (auto list.json)
</commit_message>
<xml_diff>
--- a/downloads/DMD and DPD Method Area Computation.xlsx
+++ b/downloads/DMD and DPD Method Area Computation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\CEBoardexam-randomizer\downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C8485CC-8079-41E3-A261-20321FF044F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94E0476D-C65D-4EA5-BE13-24B59C20C8DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{26CCF7B1-0108-4633-BF1D-90CD57B01C82}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{26CCF7B1-0108-4633-BF1D-90CD57B01C82}"/>
   </bookViews>
   <sheets>
     <sheet name="DPD Method" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="23">
   <si>
     <t>Departure Direction</t>
   </si>
@@ -100,6 +100,12 @@
   </si>
   <si>
     <t>DMD</t>
+  </si>
+  <si>
+    <t>2A=</t>
+  </si>
+  <si>
+    <t>A=</t>
   </si>
 </sst>
 </file>
@@ -141,9 +147,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -171,8 +180,8 @@
       <xdr:rowOff>94693</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>51289</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>785598</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>155028</xdr:rowOff>
     </xdr:to>
@@ -215,8 +224,8 @@
       <xdr:rowOff>139211</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>699440</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>346434</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>25001</xdr:rowOff>
     </xdr:to>
@@ -301,6 +310,36 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FECE641C-A3D9-479E-AED1-88F1109C0961}" name="Table1" displayName="Table1" ref="A1:I6" totalsRowShown="0">
+  <autoFilter ref="A1:I6" xr:uid="{FECE641C-A3D9-479E-AED1-88F1109C0961}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{345B454A-4099-4F7C-BB26-BC72FD22CEB7}" name="Departure Direction"/>
+    <tableColumn id="2" xr3:uid="{661409F5-3B84-4D70-850A-7DB18F85E284}" name="Latitude Direction"/>
+    <tableColumn id="3" xr3:uid="{04F6A65A-7C8E-48DE-BAA6-556792806095}" name="Bearing Angles"/>
+    <tableColumn id="4" xr3:uid="{33A15619-E474-4BCD-9934-08320028BBB8}" name="Bearing Angles in Decimal Form">
+      <calculatedColumnFormula>LEFT(C2,FIND("º",C2)-1)
+ + MID(C2,FIND("º",C2)+1,FIND("'",C2)-FIND("º",C2)-1)/60
+ + MID(C2,FIND("'",C2)+1,FIND("""",C2)-FIND("'",C2)-1)/3600</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{C4B9F5B4-E7AA-42FD-8D05-434C39856279}" name="Distances"/>
+    <tableColumn id="6" xr3:uid="{DBC321CA-6E65-4793-A0F7-AD702E2B3422}" name="Departures">
+      <calculatedColumnFormula>IF(A2="E",E2*SIN(D2*PI()/180),-E2*SIN(D2*PI()/180))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{8B26BD2A-5D70-4613-A34C-96D873AD25A5}" name="Latitudes">
+      <calculatedColumnFormula>IF(B2="N",E2*COS(D2*PI()/180),-E2*COS(D2*PI()/180))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{D944E766-E6A8-49D7-845A-9A06A004718C}" name="DPD">
+      <calculatedColumnFormula>H1+G1+G2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{84B21A31-B74B-4F5A-97A6-CA9A60BDA91F}" name="2A = DPD (Dep)">
+      <calculatedColumnFormula>H2*F2</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -622,16 +661,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82EF6EE6-AE62-426C-8C63-485618A55C97}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection sqref="A1:I8"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.42578125" customWidth="1"/>
-    <col min="2" max="2" width="32.42578125" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="28.7109375" customWidth="1"/>
+    <col min="4" max="4" width="29.28515625" customWidth="1"/>
     <col min="5" max="5" width="20.42578125" customWidth="1"/>
     <col min="6" max="6" width="15.85546875" customWidth="1"/>
     <col min="7" max="7" width="15.42578125" customWidth="1"/>
@@ -843,14 +882,17 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H7" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="I7">
         <f>SUM(I2:I6)</f>
         <v>-545171.22116134467</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H8" t="s">
-        <v>18</v>
+      <c r="H8" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="I8" s="1">
         <f>ABS(I7/2)</f>
@@ -860,6 +902,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>